<commit_message>
Fixed a bug in uploading manuscript
</commit_message>
<xml_diff>
--- a/data/spreadsheet/pilot.xlsx
+++ b/data/spreadsheet/pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collegeStuff\digitalScholarship\islam-in-china\data\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38723F11-6613-4948-8D50-1217BCD2A4CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D050187F-54B2-4B34-A2F3-3EEF57049F93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,7 +598,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished testing manuscript delete function:
</commit_message>
<xml_diff>
--- a/data/spreadsheet/pilot.xlsx
+++ b/data/spreadsheet/pilot.xlsx
@@ -436,92 +436,92 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Internal Project Id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Title in Arabic/Persian script</t>
+          <t>arab_title_script</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Transliterated Arabic Title</t>
+          <t>arab_title</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Chinese Title</t>
+          <t>chinese_title</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Author</t>
+          <t>author</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Assembler</t>
+          <t>assembler</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Editor</t>
+          <t>editor</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Scrivener</t>
+          <t>scrivener</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Translator</t>
+          <t>translator</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Type of Publication</t>
+          <t>type</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Place of Publication</t>
+          <t>place</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Publisher</t>
+          <t>publisher</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Year of Publication</t>
+          <t>year</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Standardized Year of Publication</t>
+          <t>stand_year</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>language</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Number of Pages</t>
+          <t>num_pages</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>description</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Notes</t>
+          <t>notes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Made change to spreadsheet
</commit_message>
<xml_diff>
--- a/data/spreadsheet/pilot.xlsx
+++ b/data/spreadsheet/pilot.xlsx
@@ -1058,11 +1058,7 @@
           <t>Muhammad Husayn Ibn Khalīlillāh</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Unidentified</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>Han Hucai 韩胡才</t>
@@ -1074,16 +1070,8 @@
           <t>Book</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Unidentified</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Unidentified</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
           <t>Likely 2010s</t>

</xml_diff>